<commit_message>
Modify TIM to address DH Study
- Residential and Services sector have enhanced DH options
- Four DH demand groups: Low, Medium, High and City
- New DH Supply options: Surplus heat, heat pumps, solar, & storage.
- DH cost distribution from Irish Heat Atlas
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_PWR_DH_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_PWR_DH_Trans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C726400-A589-482C-94E4-4B96034147A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D41AFBA-B753-4CC6-92D6-08D770BF7E0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="909" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="909" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="47" r:id="rId1"/>
@@ -19,6 +19,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
@@ -111,7 +112,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="84">
   <si>
     <t>IE</t>
   </si>
@@ -359,6 +359,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>https://en.wikipedia.org/wiki/ISO_3166-2:IE</t>
     </r>
@@ -790,7 +791,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{077EBEA0-2A96-405F-ACD0-787E1F6C7927}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -834,7 +835,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECF5D0B1-F3FC-42BB-B788-FD3270E3E597}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -883,7 +884,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{654E6CC1-0E51-4039-B6D4-5299F80D8846}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -933,7 +934,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B76A1BC8-0197-406B-90DE-C0A059EEFA02}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -983,7 +984,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E138389-4677-452F-B0F9-E88B25C485EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1032,7 +1033,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76901A25-C675-4DE9-82C6-E09D1F5A059C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
               <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B1489C0F-1609-4587-A5BA-D0B99739EA08}"/>
@@ -1216,62 +1217,85 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="3" refreshError="1"/>
       <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
       <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
       <sheetData sheetId="39" refreshError="1"/>
       <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="53" refreshError="1"/>
+      <sheetData sheetId="54" refreshError="1"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56" refreshError="1"/>
+      <sheetData sheetId="57" refreshError="1"/>
+      <sheetData sheetId="58" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Cover"/>
+      <sheetName val="Regions"/>
+      <sheetName val="TechSelection"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="C3" t="str">
+            <v>IE</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1601,7 +1625,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -5217,10 +5241,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B3:AA7"/>
+  <dimension ref="B3:AH7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5259,7 +5283,7 @@
     <col min="37" max="37" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -5283,7 +5307,7 @@
       <c r="Z3"/>
       <c r="AA3"/>
     </row>
-    <row r="4" spans="2:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:34" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
@@ -5303,65 +5327,178 @@
         <v>8</v>
       </c>
       <c r="H4" s="6" t="str">
-        <f>Regions!C3</f>
+        <f>[2]Regions!C3</f>
         <v>IE</v>
       </c>
-      <c r="I4" s="7" t="str">
-        <f>Regions!D3</f>
-        <v>National</v>
-      </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-      <c r="Z4"/>
-      <c r="AA4"/>
-    </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="I4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH4" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.2">
       <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="8">
         <v>1</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="8">
         <v>1</v>
       </c>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="S5"/>
-      <c r="T5"/>
-      <c r="U5"/>
-      <c r="V5"/>
-      <c r="W5"/>
-      <c r="X5"/>
-      <c r="Y5"/>
-      <c r="Z5"/>
-      <c r="AA5"/>
-    </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="J5" s="8">
+        <v>1</v>
+      </c>
+      <c r="K5" s="8">
+        <v>1</v>
+      </c>
+      <c r="L5" s="8">
+        <v>1</v>
+      </c>
+      <c r="M5" s="8">
+        <v>1</v>
+      </c>
+      <c r="N5" s="8">
+        <v>1</v>
+      </c>
+      <c r="O5" s="8">
+        <v>1</v>
+      </c>
+      <c r="P5" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>1</v>
+      </c>
+      <c r="R5" s="8">
+        <v>1</v>
+      </c>
+      <c r="S5" s="8">
+        <v>1</v>
+      </c>
+      <c r="T5" s="8">
+        <v>1</v>
+      </c>
+      <c r="U5" s="8">
+        <v>1</v>
+      </c>
+      <c r="V5" s="8">
+        <v>1</v>
+      </c>
+      <c r="W5" s="8">
+        <v>1</v>
+      </c>
+      <c r="X5" s="8">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:34" x14ac:dyDescent="0.2">
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
@@ -5381,7 +5518,7 @@
       <c r="Z6"/>
       <c r="AA6"/>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:34" x14ac:dyDescent="0.2">
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>

</xml_diff>